<commit_message>
[+1 Tarefa na Tabela]
Como não havia a tarefa de fazer o botão retornar à posição original, eu
criei e já a coloquei em desenvolvimento (na verdade eu terminei isso e
o código está funcionando).
</commit_message>
<xml_diff>
--- a/Tabela com as tarefas.xlsx
+++ b/Tabela com as tarefas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Begnini\Documents\GitHub\FabricadeRobos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naraq_000\Documents\GitHub\FabricadeRobos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4633"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>Tarefa - Nome</t>
   </si>
@@ -585,6 +585,12 @@
   </si>
   <si>
     <t>T4.07</t>
+  </si>
+  <si>
+    <t>Fazer botões de cabeça, braços e tronco retornar à posição original após o mouse soltá-los</t>
+  </si>
+  <si>
+    <t>T1.11</t>
   </si>
 </sst>
 </file>
@@ -625,7 +631,7 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -656,6 +662,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -669,7 +681,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -698,6 +710,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,9 +731,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -756,7 +771,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -828,7 +843,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -981,23 +996,23 @@
   <dimension ref="A2:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="120.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="120.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.87890625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1017,7 +1032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1028,7 +1043,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1039,7 +1054,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1050,7 +1065,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1061,7 +1076,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1072,7 +1087,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1083,7 +1098,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1094,7 +1109,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1105,7 +1120,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1116,7 +1131,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1127,17 +1142,29 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
@@ -1157,7 +1184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -1168,7 +1195,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1179,7 +1206,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1190,7 +1217,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -1201,7 +1228,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -1212,12 +1239,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="7" t="s">
         <v>0</v>
       </c>
@@ -1237,7 +1264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="10" t="s">
         <v>32</v>
       </c>
@@ -1248,7 +1275,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="10" t="s">
         <v>31</v>
       </c>
@@ -1259,7 +1286,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A31" s="10" t="s">
         <v>30</v>
       </c>
@@ -1270,7 +1297,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A32" s="10" t="s">
         <v>29</v>
       </c>
@@ -1281,7 +1308,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A33" s="3" t="s">
         <v>28</v>
       </c>
@@ -1292,7 +1319,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="s">
         <v>27</v>
       </c>
@@ -1303,7 +1330,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="s">
         <v>26</v>
       </c>
@@ -1314,7 +1341,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A36" s="4" t="s">
         <v>25</v>
       </c>
@@ -1325,12 +1352,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A39" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A40" s="7" t="s">
         <v>0</v>
       </c>
@@ -1350,7 +1377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
@@ -1361,7 +1388,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A42" s="11" t="s">
         <v>34</v>
       </c>
@@ -1372,7 +1399,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A43" s="11" t="s">
         <v>35</v>
       </c>
@@ -1383,7 +1410,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A44" s="11" t="s">
         <v>36</v>
       </c>
@@ -1394,7 +1421,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A45" s="11" t="s">
         <v>37</v>
       </c>
@@ -1405,7 +1432,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A46" s="11" t="s">
         <v>38</v>
       </c>
@@ -1416,7 +1443,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A47" s="11" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
[Criacao da Pa LUAN]
</commit_message>
<xml_diff>
--- a/Tabela com as tarefas.xlsx
+++ b/Tabela com as tarefas.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naraq_000\Documents\GitHub\FabricadeRobos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4633"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -773,7 +768,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -808,7 +803,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -985,7 +980,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -996,23 +991,23 @@
   <dimension ref="A2:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="120.5859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.87890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="120.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1043,7 +1038,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1054,7 +1049,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1065,7 +1060,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1076,18 +1071,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1098,7 +1093,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1109,7 +1104,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1120,7 +1115,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1131,7 +1126,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1142,7 +1137,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -1154,17 +1149,17 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
@@ -1184,7 +1179,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -1195,7 +1190,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1206,7 +1201,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1217,7 +1212,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -1228,7 +1223,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -1239,12 +1234,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>0</v>
       </c>
@@ -1264,7 +1259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>32</v>
       </c>
@@ -1275,7 +1270,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>31</v>
       </c>
@@ -1286,7 +1281,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>30</v>
       </c>
@@ -1297,7 +1292,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>29</v>
       </c>
@@ -1308,7 +1303,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>28</v>
       </c>
@@ -1319,7 +1314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>27</v>
       </c>
@@ -1330,7 +1325,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>26</v>
       </c>
@@ -1341,7 +1336,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>25</v>
       </c>
@@ -1352,12 +1347,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>0</v>
       </c>
@@ -1377,7 +1372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
@@ -1388,7 +1383,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>34</v>
       </c>
@@ -1399,7 +1394,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>35</v>
       </c>
@@ -1410,7 +1405,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>36</v>
       </c>
@@ -1421,7 +1416,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>37</v>
       </c>
@@ -1432,7 +1427,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>38</v>
       </c>
@@ -1443,7 +1438,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
[Tabela de Tarefa att]
</commit_message>
<xml_diff>
--- a/Tabela com as tarefas.xlsx
+++ b/Tabela com as tarefas.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Begnini\Documents\GitHub\FabricadeRobos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
   <si>
     <t>Tarefa - Nome</t>
   </si>
@@ -586,6 +591,12 @@
   </si>
   <si>
     <t>T1.11</t>
+  </si>
+  <si>
+    <t>Criar o botao de pause</t>
+  </si>
+  <si>
+    <t>T1.12</t>
   </si>
 </sst>
 </file>
@@ -980,7 +991,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -988,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F47"/>
+  <dimension ref="A2:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1056,7 @@
       <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1056,7 +1067,7 @@
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1067,7 +1078,7 @@
       <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1078,7 +1089,7 @@
       <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1089,7 +1100,7 @@
       <c r="B9" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1100,7 +1111,7 @@
       <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1111,7 +1122,7 @@
       <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1122,7 +1133,7 @@
       <c r="B12" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1145,307 +1156,315 @@
         <v>72</v>
       </c>
       <c r="C14" s="12"/>
-      <c r="D14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
-      <c r="A17" s="5" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
-      <c r="A18" s="9" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
-      <c r="A19" s="7" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B20" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C20" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F20" s="8" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
-      <c r="A20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.5">
-      <c r="A22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E41" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C48" s="6" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Att da Tabela e Jogo funcionando com o Botao de Pause]
</commit_message>
<xml_diff>
--- a/Tabela com as tarefas.xlsx
+++ b/Tabela com as tarefas.xlsx
@@ -1002,7 +1002,7 @@
   <dimension ref="A2:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1144,7 @@
       <c r="B13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1164,7 +1164,7 @@
       <c r="A15" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>